<commit_message>
Fixed reading the csvs/excel sheet
deleted the first few rows of the datasets that were unnecessary ex. last updated date and the texts "Data Source" and "World Development Indicators"
</commit_message>
<xml_diff>
--- a/data/economic-growth-indicators.xlsx
+++ b/data/economic-growth-indicators.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\asean-datascience\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E960F7-9966-4CD4-9D2C-FDA58DE531D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Growth Rate of GDP, % per Year" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="HDI" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Productivity" sheetId="3" r:id="rId6"/>
+    <sheet name="Growth Rate of GDP" sheetId="1" r:id="rId1"/>
+    <sheet name="HDI" sheetId="2" r:id="rId2"/>
+    <sheet name="Productivity" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t>Afghanistan</t>
-  </si>
-  <si>
-    <t>…</t>
   </si>
   <si>
     <t>Bangladesh</t>
@@ -111,41 +117,43 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -155,7 +163,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -171,90 +179,75 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -444,43 +437,48 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="C1" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="D1" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="E1" s="1">
-        <v>2021.0</v>
+        <v>2021</v>
       </c>
       <c r="F1" s="1">
-        <v>2022.0</v>
+        <v>2022</v>
       </c>
       <c r="G1" s="1">
-        <v>2023.0</v>
+        <v>2023</v>
       </c>
       <c r="H1" s="1">
-        <v>2024.0</v>
-      </c>
-    </row>
-    <row r="2">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -496,19 +494,13 @@
       <c r="E2" s="3">
         <v>-20.7</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
       </c>
       <c r="B3" s="3">
         <v>7.3</v>
@@ -532,9 +524,9 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3">
         <v>3.1</v>
@@ -543,24 +535,24 @@
         <v>5.8</v>
       </c>
       <c r="D4" s="3">
-        <v>-10.0</v>
+        <v>-10</v>
       </c>
       <c r="E4" s="3">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F4" s="3">
         <v>4.7</v>
       </c>
       <c r="G4" s="4">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="H4" s="4">
         <v>4.2</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3">
         <v>6.5</v>
@@ -584,9 +576,9 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3">
         <v>8.1</v>
@@ -610,9 +602,9 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3">
         <v>7.6</v>
@@ -630,15 +622,15 @@
         <v>5.8</v>
       </c>
       <c r="G7" s="4">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="H7" s="4">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3">
         <v>6.1</v>
@@ -653,27 +645,27 @@
         <v>5.7</v>
       </c>
       <c r="F8" s="3">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="G8" s="4">
         <v>0.6</v>
       </c>
       <c r="H8" s="4">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C9" s="3">
         <v>-0.2</v>
       </c>
       <c r="D9" s="3">
-        <v>-4.6</v>
+        <v>-4.5999999999999996</v>
       </c>
       <c r="E9" s="3">
         <v>3.5</v>
@@ -682,15 +674,15 @@
         <v>-7.8</v>
       </c>
       <c r="G9" s="4">
-        <v>-3.0</v>
+        <v>-3</v>
       </c>
       <c r="H9" s="4">
         <v>1.3</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3">
         <v>0.1</v>
@@ -699,7 +691,7 @@
         <v>3.9</v>
       </c>
       <c r="D10" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E10" s="3">
         <v>-1.6</v>
@@ -714,9 +706,9 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3">
         <v>7.5</v>
@@ -728,7 +720,7 @@
         <v>-3.1</v>
       </c>
       <c r="E11" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F11" s="3">
         <v>5.2</v>
@@ -737,18 +729,18 @@
         <v>5.5</v>
       </c>
       <c r="H11" s="4">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3">
         <v>5.2</v>
       </c>
       <c r="C12" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D12" s="3">
         <v>-2.1</v>
@@ -763,12 +755,12 @@
         <v>4.8</v>
       </c>
       <c r="H12" s="4">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="3">
         <v>6.2</v>
@@ -780,27 +772,27 @@
         <v>-0.5</v>
       </c>
       <c r="E13" s="3">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F13" s="3">
         <v>2.5</v>
       </c>
       <c r="G13" s="4">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="H13" s="4">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="3">
         <v>4.8</v>
       </c>
       <c r="C14" s="3">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D14" s="3">
         <v>-5.5</v>
@@ -809,18 +801,18 @@
         <v>3.1</v>
       </c>
       <c r="F14" s="3">
-        <v>8.7</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="G14" s="4">
         <v>4.7</v>
       </c>
       <c r="H14" s="4">
-        <v>4.9</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="3">
         <v>6.4</v>
@@ -835,7 +827,7 @@
         <v>-5.9</v>
       </c>
       <c r="F15" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G15" s="4">
         <v>2.8</v>
@@ -844,9 +836,9 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="3">
         <v>6.3</v>
@@ -864,15 +856,15 @@
         <v>7.6</v>
       </c>
       <c r="G16" s="4">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="H16" s="4">
         <v>6.2</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="3">
         <v>3.6</v>
@@ -890,15 +882,15 @@
         <v>3.6</v>
       </c>
       <c r="G17" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="H17" s="4">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="3">
         <v>4.2</v>
@@ -922,9 +914,9 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="3">
         <v>-0.7</v>
@@ -933,7 +925,7 @@
         <v>2.1</v>
       </c>
       <c r="D19" s="3">
-        <v>-8.3</v>
+        <v>-8.3000000000000007</v>
       </c>
       <c r="E19" s="3">
         <v>2.9</v>
@@ -945,12 +937,12 @@
         <v>3.1</v>
       </c>
       <c r="H19" s="4">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="3">
         <v>7.5</v>
@@ -965,7 +957,7 @@
         <v>2.6</v>
       </c>
       <c r="F20" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="G20" s="4">
         <v>6.5</v>
@@ -975,103 +967,110 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.25"/>
-    <col customWidth="1" min="2" max="5" width="12.88"/>
+    <col min="1" max="1" width="21.26953125" customWidth="1"/>
+    <col min="2" max="2" width="9.36328125" customWidth="1"/>
+    <col min="3" max="3" width="9.26953125" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" customWidth="1"/>
+    <col min="5" max="5" width="9.90625" customWidth="1"/>
+    <col min="6" max="6" width="16.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:12" ht="70" x14ac:dyDescent="0.3">
       <c r="B1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="8">
-        <v>0.483</v>
+        <v>0.48299999999999998</v>
       </c>
       <c r="C2" s="8">
-        <v>0.488</v>
+        <v>0.48799999999999999</v>
       </c>
       <c r="D2" s="8">
-        <v>0.483</v>
+        <v>0.48299999999999998</v>
       </c>
       <c r="E2" s="9">
-        <v>0.478</v>
+        <v>0.47799999999999998</v>
       </c>
       <c r="F2" s="9">
-        <v>62.0</v>
+        <v>62</v>
       </c>
       <c r="G2" s="9">
         <v>10.3</v>
       </c>
       <c r="H2" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="I2" s="10">
-        <v>1824.0</v>
+        <v>1824</v>
       </c>
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
       <c r="L2" s="8"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="8">
-        <v>0.635</v>
+        <v>0.63500000000000001</v>
       </c>
       <c r="C3" s="8">
-        <v>0.644</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="D3" s="8">
-        <v>0.655</v>
+        <v>0.65500000000000003</v>
       </c>
       <c r="E3" s="9">
-        <v>0.661</v>
+        <v>0.66100000000000003</v>
       </c>
       <c r="F3" s="9">
-        <v>72.4</v>
+        <v>72.400000000000006</v>
       </c>
       <c r="G3" s="9">
         <v>12.4</v>
@@ -1080,27 +1079,27 @@
         <v>7.4</v>
       </c>
       <c r="I3" s="10">
-        <v>5472.0</v>
+        <v>5472</v>
       </c>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
       <c r="L3" s="8"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="8">
-        <v>0.658</v>
+        <v>0.65800000000000003</v>
       </c>
       <c r="C4" s="8">
-        <v>0.671</v>
+        <v>0.67100000000000004</v>
       </c>
       <c r="D4" s="8">
-        <v>0.668</v>
+        <v>0.66800000000000004</v>
       </c>
       <c r="E4" s="9">
-        <v>0.666</v>
+        <v>0.66600000000000004</v>
       </c>
       <c r="F4" s="9">
         <v>71.8</v>
@@ -1112,27 +1111,27 @@
         <v>5.2</v>
       </c>
       <c r="I4" s="10">
-        <v>9438.0</v>
+        <v>9438</v>
       </c>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" s="8"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="8">
-        <v>0.645</v>
+        <v>0.64500000000000002</v>
       </c>
       <c r="C5" s="8">
-        <v>0.645</v>
+        <v>0.64500000000000002</v>
       </c>
       <c r="D5" s="8">
-        <v>0.642</v>
+        <v>0.64200000000000002</v>
       </c>
       <c r="E5" s="9">
-        <v>0.633</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="F5" s="9">
         <v>67.2</v>
@@ -1144,15 +1143,15 @@
         <v>6.7</v>
       </c>
       <c r="I5" s="10">
-        <v>6590.0</v>
+        <v>6590</v>
       </c>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
       <c r="L5" s="8"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="8">
         <v>0.75</v>
@@ -1161,13 +1160,13 @@
         <v>0.755</v>
       </c>
       <c r="D6" s="8">
-        <v>0.734</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="E6" s="9">
         <v>0.747</v>
       </c>
       <c r="F6" s="9">
-        <v>79.9</v>
+        <v>79.900000000000006</v>
       </c>
       <c r="G6" s="9">
         <v>12.6</v>
@@ -1176,94 +1175,94 @@
         <v>7.3</v>
       </c>
       <c r="I6" s="10">
-        <v>15448.0</v>
+        <v>15448</v>
       </c>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
       <c r="L6" s="8"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="8">
-        <v>0.601</v>
+        <v>0.60099999999999998</v>
       </c>
       <c r="C7" s="8">
-        <v>0.611</v>
+        <v>0.61099999999999999</v>
       </c>
       <c r="D7" s="8">
-        <v>0.604</v>
+        <v>0.60399999999999998</v>
       </c>
       <c r="E7" s="9">
-        <v>0.602</v>
+        <v>0.60199999999999998</v>
       </c>
       <c r="F7" s="9">
-        <v>68.4</v>
+        <v>68.400000000000006</v>
       </c>
       <c r="G7" s="9">
         <v>12.9</v>
       </c>
       <c r="H7" s="9">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I7" s="10">
-        <v>3877.0</v>
+        <v>3877</v>
       </c>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
       <c r="L7" s="8"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="8">
-        <v>0.545</v>
+        <v>0.54500000000000004</v>
       </c>
       <c r="C8" s="8">
-        <v>0.546</v>
+        <v>0.54600000000000004</v>
       </c>
       <c r="D8" s="8">
-        <v>0.543</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="E8" s="9">
-        <v>0.544</v>
+        <v>0.54400000000000004</v>
       </c>
       <c r="F8" s="9">
-        <v>66.1</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="G8" s="9">
-        <v>8.7</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="H8" s="9">
         <v>4.5</v>
       </c>
       <c r="I8" s="10">
-        <v>4624.0</v>
+        <v>4624</v>
       </c>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
       <c r="L8" s="8"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="8">
-        <v>0.776</v>
+        <v>0.77600000000000002</v>
       </c>
       <c r="C9" s="8">
-        <v>0.778</v>
+        <v>0.77800000000000002</v>
       </c>
       <c r="D9" s="8">
         <v>0.78</v>
       </c>
       <c r="E9" s="9">
-        <v>0.782</v>
+        <v>0.78200000000000003</v>
       </c>
       <c r="F9" s="9">
-        <v>76.4</v>
+        <v>76.400000000000006</v>
       </c>
       <c r="G9" s="9">
         <v>14.1</v>
@@ -1272,13 +1271,13 @@
         <v>10.8</v>
       </c>
       <c r="I9" s="10">
-        <v>12578.0</v>
+        <v>12578</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
       <c r="L9" s="8"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -1292,9 +1291,9 @@
       <c r="K10" s="11"/>
       <c r="L10" s="8"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="8">
         <v>0.83</v>
@@ -1306,71 +1305,71 @@
         <v>0.83</v>
       </c>
       <c r="E11" s="9">
-        <v>0.829</v>
+        <v>0.82899999999999996</v>
       </c>
       <c r="F11" s="9">
-        <v>74.6</v>
+        <v>74.599999999999994</v>
       </c>
       <c r="G11" s="9">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="H11" s="9">
-        <v>9.2</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="I11" s="10">
-        <v>64490.0</v>
+        <v>64490</v>
       </c>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
       <c r="L11" s="8"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="8">
-        <v>0.591</v>
+        <v>0.59099999999999997</v>
       </c>
       <c r="C12" s="8">
-        <v>0.598</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="D12" s="8">
-        <v>0.596</v>
+        <v>0.59599999999999997</v>
       </c>
       <c r="E12" s="9">
-        <v>0.593</v>
+        <v>0.59299999999999997</v>
       </c>
       <c r="F12" s="9">
-        <v>69.6</v>
+        <v>69.599999999999994</v>
       </c>
       <c r="G12" s="9">
         <v>11.5</v>
       </c>
       <c r="H12" s="9">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I12" s="10">
-        <v>4079.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>4079</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="8">
         <v>0.71</v>
       </c>
       <c r="C13" s="8">
-        <v>0.716</v>
+        <v>0.71599999999999997</v>
       </c>
       <c r="D13" s="8">
-        <v>0.709</v>
+        <v>0.70899999999999996</v>
       </c>
       <c r="E13" s="9">
-        <v>0.705</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="F13" s="9">
-        <v>67.6</v>
+        <v>67.599999999999994</v>
       </c>
       <c r="G13" s="9">
         <v>13.7</v>
@@ -1379,27 +1378,27 @@
         <v>8.6</v>
       </c>
       <c r="I13" s="10">
-        <v>11466.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>11466</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="8">
-        <v>0.607</v>
+        <v>0.60699999999999998</v>
       </c>
       <c r="C14" s="8">
         <v>0.61</v>
       </c>
       <c r="D14" s="8">
-        <v>0.608</v>
+        <v>0.60799999999999998</v>
       </c>
       <c r="E14" s="9">
-        <v>0.607</v>
+        <v>0.60699999999999998</v>
       </c>
       <c r="F14" s="9">
-        <v>68.1</v>
+        <v>68.099999999999994</v>
       </c>
       <c r="G14" s="9">
         <v>10.1</v>
@@ -1408,27 +1407,27 @@
         <v>5.4</v>
       </c>
       <c r="I14" s="10">
-        <v>7700.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>7700</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="8">
-        <v>0.807</v>
+        <v>0.80700000000000005</v>
       </c>
       <c r="C15" s="8">
         <v>0.81</v>
       </c>
       <c r="D15" s="8">
-        <v>0.806</v>
+        <v>0.80600000000000005</v>
       </c>
       <c r="E15" s="9">
-        <v>0.803</v>
+        <v>0.80300000000000005</v>
       </c>
       <c r="F15" s="9">
-        <v>74.9</v>
+        <v>74.900000000000006</v>
       </c>
       <c r="G15" s="9">
         <v>13.3</v>
@@ -1437,24 +1436,24 @@
         <v>10.6</v>
       </c>
       <c r="I15" s="10">
-        <v>26658.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>26658</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="8">
         <v>0.59</v>
       </c>
       <c r="C16" s="8">
-        <v>0.598</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="D16" s="8">
         <v>0.6</v>
       </c>
       <c r="E16" s="9">
-        <v>0.585</v>
+        <v>0.58499999999999996</v>
       </c>
       <c r="F16" s="9">
         <v>65.7</v>
@@ -1466,24 +1465,24 @@
         <v>6.4</v>
       </c>
       <c r="I16" s="10">
-        <v>3851.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>3851</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="14" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="8">
         <v>0.71</v>
       </c>
       <c r="C17" s="8">
-        <v>0.718</v>
+        <v>0.71799999999999997</v>
       </c>
       <c r="D17" s="8">
         <v>0.71</v>
       </c>
       <c r="E17" s="9">
-        <v>0.699</v>
+        <v>0.69899999999999995</v>
       </c>
       <c r="F17" s="9">
         <v>69.3</v>
@@ -1492,27 +1491,27 @@
         <v>13.1</v>
       </c>
       <c r="H17" s="9">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="I17" s="10">
-        <v>8920.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>8920</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="14" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="8">
         <v>0.94</v>
       </c>
       <c r="C18" s="8">
-        <v>0.943</v>
+        <v>0.94299999999999995</v>
       </c>
       <c r="D18" s="8">
-        <v>0.939</v>
+        <v>0.93899999999999995</v>
       </c>
       <c r="E18" s="9">
-        <v>0.939</v>
+        <v>0.93899999999999995</v>
       </c>
       <c r="F18" s="9">
         <v>82.8</v>
@@ -1524,21 +1523,21 @@
         <v>11.9</v>
       </c>
       <c r="I18" s="10">
-        <v>90919.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>90919</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="14" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="8">
-        <v>0.795</v>
+        <v>0.79500000000000004</v>
       </c>
       <c r="C19" s="8">
-        <v>0.804</v>
+        <v>0.80400000000000005</v>
       </c>
       <c r="D19" s="8">
-        <v>0.802</v>
+        <v>0.80200000000000005</v>
       </c>
       <c r="E19" s="9">
         <v>0.8</v>
@@ -1550,27 +1549,27 @@
         <v>15.9</v>
       </c>
       <c r="H19" s="9">
-        <v>8.7</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="I19" s="10">
-        <v>17030.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>17030</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="14" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="8">
-        <v>0.605</v>
+        <v>0.60499999999999998</v>
       </c>
       <c r="C20" s="8">
-        <v>0.614</v>
+        <v>0.61399999999999999</v>
       </c>
       <c r="D20" s="8">
-        <v>0.614</v>
+        <v>0.61399999999999999</v>
       </c>
       <c r="E20" s="9">
-        <v>0.607</v>
+        <v>0.60699999999999998</v>
       </c>
       <c r="F20" s="9">
         <v>67.7</v>
@@ -1582,39 +1581,39 @@
         <v>5.4</v>
       </c>
       <c r="I20" s="10">
-        <v>4461.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="14" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="8">
-        <v>0.697</v>
+        <v>0.69699999999999995</v>
       </c>
       <c r="C21" s="8">
-        <v>0.703</v>
+        <v>0.70299999999999996</v>
       </c>
       <c r="D21" s="8">
         <v>0.71</v>
       </c>
       <c r="E21" s="9">
-        <v>0.703</v>
+        <v>0.70299999999999996</v>
       </c>
       <c r="F21" s="9">
-        <v>73.6</v>
+        <v>73.599999999999994</v>
       </c>
       <c r="G21" s="9">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="H21" s="9">
         <v>8.4</v>
       </c>
       <c r="I21" s="10">
-        <v>7867.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>7867</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="14" x14ac:dyDescent="0.3">
       <c r="A22" s="12"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -1625,7 +1624,7 @@
       <c r="H22" s="8"/>
       <c r="I22" s="13"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:9" ht="14" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -1636,7 +1635,7 @@
       <c r="H23" s="8"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:9" ht="14" x14ac:dyDescent="0.3">
       <c r="A24" s="12"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -1647,7 +1646,7 @@
       <c r="H24" s="8"/>
       <c r="I24" s="13"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:9" ht="14" x14ac:dyDescent="0.3">
       <c r="A25" s="12"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -1658,7 +1657,7 @@
       <c r="H25" s="8"/>
       <c r="I25" s="13"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:9" ht="14" x14ac:dyDescent="0.3">
       <c r="A26" s="12"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -1669,7 +1668,7 @@
       <c r="H26" s="8"/>
       <c r="I26" s="13"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:9" ht="14" x14ac:dyDescent="0.3">
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -1679,7 +1678,7 @@
       <c r="H27" s="8"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:9" ht="14" x14ac:dyDescent="0.3">
       <c r="A28" s="12"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -1690,7 +1689,7 @@
       <c r="H28" s="8"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:9" ht="14" x14ac:dyDescent="0.3">
       <c r="A29" s="12"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -1701,7 +1700,7 @@
       <c r="H29" s="8"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:9" ht="14" x14ac:dyDescent="0.3">
       <c r="A30" s="12"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -1712,7 +1711,7 @@
       <c r="H30" s="8"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:9" ht="14" x14ac:dyDescent="0.3">
       <c r="A31" s="12"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -1724,278 +1723,279 @@
       <c r="I31" s="13"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="14">
-        <v>2016.0</v>
-      </c>
-      <c r="C1" s="14">
-        <v>2017.0</v>
-      </c>
-      <c r="D1" s="14">
-        <v>2018.0</v>
-      </c>
-      <c r="E1" s="14">
-        <v>2019.0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="14">
-        <v>4.113085</v>
-      </c>
-      <c r="C2" s="14">
-        <v>4.307637</v>
-      </c>
-      <c r="D2" s="14">
-        <v>4.59153</v>
-      </c>
-      <c r="E2" s="14">
-        <v>4.791032</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="16">
-        <v>7.609988</v>
-      </c>
-      <c r="C3" s="17">
-        <v>8.009788</v>
-      </c>
-      <c r="D3" s="17">
-        <v>8.536673</v>
-      </c>
-      <c r="E3" s="14">
-        <v>8.680879</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="15" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4.1130849999999999</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4.3076369999999997</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4.5915299999999997</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4.7910320000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="14">
+        <v>7.6099880000000004</v>
+      </c>
+      <c r="C3" s="15">
+        <v>8.0097880000000004</v>
+      </c>
+      <c r="D3" s="15">
+        <v>8.5366730000000004</v>
+      </c>
+      <c r="E3" s="1">
+        <v>8.6808789999999991</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="14">
+        <v>7.953004</v>
+      </c>
+      <c r="C4" s="15">
+        <v>8.3222070000000006</v>
+      </c>
+      <c r="D4" s="15">
+        <v>8.6686979999999991</v>
+      </c>
+      <c r="E4" s="1">
+        <v>8.7724130000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="16">
-        <v>7.953004</v>
-      </c>
-      <c r="C4" s="17">
-        <v>8.322207</v>
-      </c>
-      <c r="D4" s="17">
-        <v>8.668698</v>
-      </c>
-      <c r="E4" s="14">
-        <v>8.772413</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="15">
-        <v>17.27541</v>
-      </c>
-      <c r="C5" s="17">
+      <c r="B5" s="14">
+        <v>17.275410000000001</v>
+      </c>
+      <c r="C5" s="15">
         <v>17.04851</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="15">
         <v>17.89124</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="1">
         <v>18.01952</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="14">
+        <v>2.8283130000000001</v>
+      </c>
+      <c r="C6" s="15">
+        <v>3.0226500000000001</v>
+      </c>
+      <c r="D6" s="15">
+        <v>3.2637420000000001</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3.4332099999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="15">
-        <v>2.828313</v>
-      </c>
-      <c r="C6" s="17">
-        <v>3.02265</v>
-      </c>
-      <c r="D6" s="17">
-        <v>3.263742</v>
-      </c>
-      <c r="E6" s="14">
-        <v>3.43321</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="16">
+      <c r="B7" s="14">
         <v>11.20515</v>
       </c>
-      <c r="C7" s="17">
-        <v>11.35479</v>
-      </c>
-      <c r="D7" s="17">
-        <v>11.73003</v>
-      </c>
-      <c r="E7" s="14">
+      <c r="C7" s="15">
+        <v>11.354789999999999</v>
+      </c>
+      <c r="D7" s="15">
+        <v>11.730029999999999</v>
+      </c>
+      <c r="E7" s="1">
         <v>11.84327</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="14">
+        <v>23.226150000000001</v>
+      </c>
+      <c r="C8" s="15">
+        <v>23.65408</v>
+      </c>
+      <c r="D8" s="15">
+        <v>24.144670000000001</v>
+      </c>
+      <c r="E8" s="1">
+        <v>24.754380000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="16">
-        <v>23.22615</v>
-      </c>
-      <c r="C8" s="17">
-        <v>23.65408</v>
-      </c>
-      <c r="D8" s="17">
-        <v>24.14467</v>
-      </c>
-      <c r="E8" s="14">
-        <v>24.75438</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="15" t="s">
+      <c r="B9" s="14">
+        <v>4.7110110000000001</v>
+      </c>
+      <c r="C9" s="15">
+        <v>4.7354839999999996</v>
+      </c>
+      <c r="D9" s="15">
+        <v>4.7745119999999996</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5.1479140000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="16">
-        <v>4.711011</v>
-      </c>
-      <c r="C9" s="17">
-        <v>4.735484</v>
-      </c>
-      <c r="D9" s="17">
-        <v>4.774512</v>
-      </c>
-      <c r="E9" s="14">
-        <v>5.147914</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="15" t="s">
+      <c r="B10" s="14">
+        <v>8.8495799999999996</v>
+      </c>
+      <c r="C10" s="15">
+        <v>9.45045</v>
+      </c>
+      <c r="D10" s="15">
+        <v>9.8356320000000004</v>
+      </c>
+      <c r="E10" s="1">
+        <v>9.9296810000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="16">
-        <v>8.84958</v>
-      </c>
-      <c r="C10" s="17">
-        <v>9.45045</v>
-      </c>
-      <c r="D10" s="17">
-        <v>9.835632</v>
-      </c>
-      <c r="E10" s="14">
-        <v>9.929681</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="15" t="s">
+      <c r="B11" s="14">
+        <v>49.459690000000002</v>
+      </c>
+      <c r="C11" s="15">
+        <v>54.298780000000001</v>
+      </c>
+      <c r="D11" s="15">
+        <v>55.625140000000002</v>
+      </c>
+      <c r="E11" s="1">
+        <v>54.552579999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="16">
-        <v>49.45969</v>
-      </c>
-      <c r="C11" s="17">
-        <v>54.29878</v>
-      </c>
-      <c r="D11" s="17">
-        <v>55.62514</v>
-      </c>
-      <c r="E11" s="14">
-        <v>54.55258</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="16">
-        <v>13.13573</v>
-      </c>
-      <c r="C12" s="17">
-        <v>14.74584</v>
-      </c>
-      <c r="D12" s="17">
-        <v>14.85936</v>
-      </c>
-      <c r="E12" s="14">
+      <c r="B12" s="14">
+        <v>13.135730000000001</v>
+      </c>
+      <c r="C12" s="15">
+        <v>14.745839999999999</v>
+      </c>
+      <c r="D12" s="15">
+        <v>14.859360000000001</v>
+      </c>
+      <c r="E12" s="1">
         <v>15.16723</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="17">
-        <v>5.156925</v>
-      </c>
-      <c r="C13" s="17">
-        <v>5.652919</v>
-      </c>
-      <c r="D13" s="17">
-        <v>5.982665</v>
-      </c>
-      <c r="E13" s="14">
-        <v>6.739149</v>
-      </c>
-    </row>
-    <row r="14">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="15">
+        <v>5.1569250000000002</v>
+      </c>
+      <c r="C13" s="15">
+        <v>5.6529189999999998</v>
+      </c>
+      <c r="D13" s="15">
+        <v>5.9826649999999999</v>
+      </c>
+      <c r="E13" s="1">
+        <v>6.7391490000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-    </row>
-    <row r="15">
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-    </row>
-    <row r="16">
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-    </row>
-    <row r="17">
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-    </row>
-    <row r="18">
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-    </row>
-    <row r="19">
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-    </row>
-    <row r="20">
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added East Asian Countries to Econ Growth Indicators
</commit_message>
<xml_diff>
--- a/data/economic-growth-indicators.xlsx
+++ b/data/economic-growth-indicators.xlsx
@@ -8,21 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\asean-datascience\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7B977F-D86A-4780-9545-99CDC2D07F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701071AB-EF75-42EA-819C-CFBC8D9B6FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Growth Rate of GDP" sheetId="1" r:id="rId1"/>
     <sheet name="HDI" sheetId="2" r:id="rId2"/>
     <sheet name="Productivity" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="36">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -112,17 +125,48 @@
   </si>
   <si>
     <t>Vietnam</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>Taipei,China</t>
+  </si>
+  <si>
+    <t>Hong Kong SAR, China</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Korea, Rep.</t>
+  </si>
+  <si>
+    <t>Japan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="4">
+    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="169" formatCode="#,###,##0.000"/>
+    <numFmt numFmtId="170" formatCode="#,###,##0.0"/>
+    <numFmt numFmtId="171" formatCode="#,###,##0"/>
+  </numFmts>
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -157,8 +201,43 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,6 +256,18 @@
         <bgColor rgb="FFC1F3FF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEFFCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC1F3FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -187,51 +278,133 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="12" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="12" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="12" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{05DDA452-CB6E-4C64-B277-F9C6657F57F0}"/>
+    <cellStyle name="Normal 2 2" xfId="4" xr:uid="{9C0CC116-8087-42C5-A9A1-1B3AEBDF3759}"/>
+    <cellStyle name="Normal 2 3" xfId="3" xr:uid="{A7280E4C-C764-4679-ACC6-3FF3D7E2E11F}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{D0600008-9D7F-455E-B12B-3770BE0867A2}"/>
+    <cellStyle name="Normal 4" xfId="5" xr:uid="{E2559894-F7B2-4082-934A-04A2FD6A89EC}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -447,10 +620,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -966,8 +1139,139 @@
         <v>6.8</v>
       </c>
     </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="16">
+        <v>2.846877928228146</v>
+      </c>
+      <c r="C21" s="16">
+        <v>-1.6723903457560065</v>
+      </c>
+      <c r="D21" s="16">
+        <v>-6.5447812957751204</v>
+      </c>
+      <c r="E21" s="16">
+        <v>6.4479576708661694</v>
+      </c>
+      <c r="F21" s="16">
+        <v>-3.5070411508229218</v>
+      </c>
+      <c r="G21" s="17">
+        <v>3.6000000000000054</v>
+      </c>
+      <c r="H21" s="17">
+        <v>3.700000000000006</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="16">
+        <v>7.7</v>
+      </c>
+      <c r="C22" s="16">
+        <v>5.6</v>
+      </c>
+      <c r="D22" s="16">
+        <v>-4.5999999999999996</v>
+      </c>
+      <c r="E22" s="16">
+        <v>1.6</v>
+      </c>
+      <c r="F22" s="16">
+        <v>4.8</v>
+      </c>
+      <c r="G22" s="17">
+        <v>5.4</v>
+      </c>
+      <c r="H22" s="17">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="16">
+        <v>6.72614540067904</v>
+      </c>
+      <c r="C23" s="16">
+        <v>6.0732535162232315</v>
+      </c>
+      <c r="D23" s="16">
+        <v>2.146864581367347</v>
+      </c>
+      <c r="E23" s="16">
+        <v>8.4</v>
+      </c>
+      <c r="F23" s="16">
+        <v>3</v>
+      </c>
+      <c r="G23" s="17">
+        <v>5.0225323399166744</v>
+      </c>
+      <c r="H23" s="17">
+        <v>4.4507251172227758</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="16">
+        <v>2.9074037737713443</v>
+      </c>
+      <c r="C24" s="16">
+        <v>2.2439778601101246</v>
+      </c>
+      <c r="D24" s="16">
+        <v>-0.70941535939766931</v>
+      </c>
+      <c r="E24" s="16">
+        <v>4.1453239543092435</v>
+      </c>
+      <c r="F24" s="16">
+        <v>2.6</v>
+      </c>
+      <c r="G24" s="17">
+        <v>1.4999999999999902</v>
+      </c>
+      <c r="H24" s="17">
+        <v>2.200000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="16">
+        <v>2.7867698826940401</v>
+      </c>
+      <c r="C25" s="16">
+        <v>3.0639500646228557</v>
+      </c>
+      <c r="D25" s="16">
+        <v>3.3866359350104958</v>
+      </c>
+      <c r="E25" s="16">
+        <v>6.5276632552648151</v>
+      </c>
+      <c r="F25" s="16">
+        <v>2.4523589302419824</v>
+      </c>
+      <c r="G25" s="17">
+        <v>2.0000000000000018</v>
+      </c>
+      <c r="H25" s="17">
+        <v>2.6000000000000023</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -978,8 +1282,8 @@
   </sheetPr>
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1483,7 +1787,7 @@
         <v>8920</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
@@ -1512,7 +1816,7 @@
         <v>90919</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>16</v>
       </c>
@@ -1541,7 +1845,7 @@
         <v>17030</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>17</v>
       </c>
@@ -1570,7 +1874,7 @@
         <v>4461</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>29</v>
       </c>
@@ -1599,51 +1903,125 @@
         <v>7867</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="14" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="13"/>
-    </row>
-    <row r="22" spans="1:9" ht="14" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="13"/>
-    </row>
-    <row r="23" spans="1:9" ht="14" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="13"/>
-    </row>
-    <row r="24" spans="1:9" ht="14" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="13"/>
-    </row>
-    <row r="25" spans="1:9" ht="14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="14" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="25">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="C21" s="25">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="D21" s="25">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="E21" s="21">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="F21" s="22">
+        <v>85.473399999999998</v>
+      </c>
+      <c r="G21" s="22">
+        <v>17.278169630000001</v>
+      </c>
+      <c r="H21" s="22">
+        <v>12.22620964</v>
+      </c>
+      <c r="I21" s="23">
+        <v>62606.845399999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="14" x14ac:dyDescent="0.3">
+      <c r="A22" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="29">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="C22" s="29">
+        <v>0.746</v>
+      </c>
+      <c r="D22" s="29">
+        <v>0.745</v>
+      </c>
+      <c r="E22" s="26">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="F22" s="27">
+        <v>70.975399999999993</v>
+      </c>
+      <c r="G22" s="27">
+        <v>14.980349540000001</v>
+      </c>
+      <c r="H22" s="27">
+        <v>9.4237003329999993</v>
+      </c>
+      <c r="I22" s="28">
+        <v>10588.22532</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="14" x14ac:dyDescent="0.3">
+      <c r="A23" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="36">
+        <v>0.755</v>
+      </c>
+      <c r="C23" s="36">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="D23" s="36">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="E23" s="32">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="F23" s="33">
+        <v>78.210700000000003</v>
+      </c>
+      <c r="G23" s="33">
+        <v>14.2361149</v>
+      </c>
+      <c r="H23" s="33">
+        <v>7.6001184459999998</v>
+      </c>
+      <c r="I23" s="34">
+        <v>17504.399689999998</v>
+      </c>
+      <c r="J23" s="20"/>
+      <c r="L23" s="20"/>
+    </row>
+    <row r="24" spans="1:12" ht="14" x14ac:dyDescent="0.3">
+      <c r="A24" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="43">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="C24" s="43">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="D24" s="43">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="E24" s="39">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="F24" s="40">
+        <v>83.697800000000001</v>
+      </c>
+      <c r="G24" s="40">
+        <v>16.521739960000001</v>
+      </c>
+      <c r="H24" s="40">
+        <v>12.51293027</v>
+      </c>
+      <c r="I24" s="41">
+        <v>44500.93187</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A25" s="12"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -1654,17 +2032,14 @@
       <c r="H25" s="8"/>
       <c r="I25" s="13"/>
     </row>
-    <row r="26" spans="1:9" ht="14" x14ac:dyDescent="0.3">
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="13"/>
-    </row>
-    <row r="27" spans="1:9" ht="14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="H26" s="30"/>
+      <c r="J26" s="31"/>
+      <c r="L26" s="31"/>
+    </row>
+    <row r="27" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A27" s="12"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -1675,18 +2050,15 @@
       <c r="H27" s="8"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="1:9" ht="14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A28" s="12"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="13"/>
-    </row>
-    <row r="29" spans="1:9" ht="14" x14ac:dyDescent="0.3">
+      <c r="C28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="H28" s="37"/>
+      <c r="J28" s="37"/>
+      <c r="L28" s="38"/>
+    </row>
+    <row r="29" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A29" s="12"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -1697,7 +2069,7 @@
       <c r="H29" s="8"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="1:9" ht="14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="14" x14ac:dyDescent="0.3">
       <c r="A30" s="12"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -1720,7 +2092,9 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1943,42 +2317,87 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="7"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
+      <c r="A14" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="15">
+        <v>44.553089999999997</v>
+      </c>
+      <c r="C14" s="15">
+        <v>44.372982</v>
+      </c>
+      <c r="D14" s="15">
+        <v>49.249600000000001</v>
+      </c>
+      <c r="E14">
+        <v>49.118411999999999</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="7"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
+      <c r="A15" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="15">
+        <v>10.742945000000001</v>
+      </c>
+      <c r="C15" s="15">
+        <v>11.3577385</v>
+      </c>
+      <c r="D15" s="15">
+        <v>11.380233</v>
+      </c>
+      <c r="E15">
+        <v>11.692401</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="7"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="7"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="15">
+        <v>36.877330000000001</v>
+      </c>
+      <c r="C16" s="15">
+        <v>39.083927000000003</v>
+      </c>
+      <c r="D16" s="15">
+        <v>40.092373000000002</v>
+      </c>
+      <c r="E16">
+        <v>40.768528000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="15">
+        <v>42.681710000000002</v>
+      </c>
+      <c r="C17" s="15">
+        <v>42.422935000000003</v>
+      </c>
+      <c r="D17">
+        <v>41.737830000000002</v>
+      </c>
+      <c r="E17">
+        <v>42.564120000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
     </row>
   </sheetData>

</xml_diff>